<commit_message>
testes usabilidade + fix last things
</commit_message>
<xml_diff>
--- a/testes-usabilidade/Grelha_Observacao_Testes_Usabilidade.xlsx
+++ b/testes-usabilidade/Grelha_Observacao_Testes_Usabilidade.xlsx
@@ -1,36 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Stuff\UM\A4_S2\AA-SIC\aa-sic-2425\testes-usabilidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BC6741-B877-4A71-8A36-7344321B43E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53599A05-FCE1-4498-8AF1-8ED49A7DE2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TesteCliente1" sheetId="1" r:id="rId1"/>
     <sheet name="TesteCliente2" sheetId="3" r:id="rId2"/>
     <sheet name="TesteCliente3" sheetId="4" r:id="rId3"/>
-    <sheet name="TesteOwner" sheetId="5" r:id="rId4"/>
+    <sheet name="TesteOwner1" sheetId="5" r:id="rId4"/>
+    <sheet name="TesteOwner2" sheetId="6" r:id="rId5"/>
+    <sheet name="TesteOwner3" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
   <si>
     <t>Tarefa</t>
   </si>
   <si>
-    <t>Tempo (min:seg)</t>
-  </si>
-  <si>
     <t>Dificuldades Observadas</t>
   </si>
   <si>
@@ -49,21 +48,12 @@
     <t>Observações Gerais:</t>
   </si>
   <si>
-    <t>- Comportamentos não verbais:</t>
-  </si>
-  <si>
-    <t>- Comentários espontâneos:</t>
-  </si>
-  <si>
     <t>- Sugestões do utilizador:</t>
   </si>
   <si>
     <t>- Erros recorrentes:</t>
   </si>
   <si>
-    <t>- Observações adicionais:</t>
-  </si>
-  <si>
     <t>Notas</t>
   </si>
   <si>
@@ -74,13 +64,124 @@
   </si>
   <si>
     <t>4. Rejeitar reserva</t>
+  </si>
+  <si>
+    <t>Rápido</t>
+  </si>
+  <si>
+    <t>Um bocado lento, não foi à página desejada</t>
+  </si>
+  <si>
+    <t>Rápido e intuitivo , teve uma resposta lenta ao número de slots</t>
+  </si>
+  <si>
+    <t>Lento</t>
+  </si>
+  <si>
+    <t>Tive que indicar que um owner é um user e que devia procurar outra view</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Não conseguiu perceber que era para ir à enterprise view</t>
+  </si>
+  <si>
+    <t>Nada.</t>
+  </si>
+  <si>
+    <t>Nenhum.</t>
+  </si>
+  <si>
+    <t>Não encontrou facilmente os botões da nav bar</t>
+  </si>
+  <si>
+    <t>Simples.</t>
+  </si>
+  <si>
+    <t>Por especificar a track na tarefa ele associa em ir ver às tracks em vez de às sessões.</t>
+  </si>
+  <si>
+    <t>Não conseguiu perceber o erro que tinha de estar nos participantes para fazer a reserva. Bom feedback de sucesso após criar a reserva.</t>
+  </si>
+  <si>
+    <t>Lento por falha de escrita</t>
+  </si>
+  <si>
+    <t>Leu mal o email do guião, mas percebeu rapidamente o erro com o feedback do site.</t>
+  </si>
+  <si>
+    <t>Demorou a perceber qual era a sessão pretendida.</t>
+  </si>
+  <si>
+    <t>Pensou que nas sessões conseguia ver todas e não apenas as suas.</t>
+  </si>
+  <si>
+    <t>Má instrução da tarefa. Deu a entender que ele próprio não devia estar incluído nos participants.</t>
+  </si>
+  <si>
+    <t>Perceber que ele era o user "test" que já estava adicionado aos participants</t>
+  </si>
+  <si>
+    <t>A ordem das sessões podia estar mais explícita ou até ter filtros/ordenação.</t>
+  </si>
+  <si>
+    <t>Clarificar a ordem das sessões, adicionar filtros. Nos detalhes da reserva mostrar o dia da semana ao lado da data.</t>
+  </si>
+  <si>
+    <t>Médio.</t>
+  </si>
+  <si>
+    <t>Fez a reserva para o dia errado. Percebeu bem que o user "test" era ele.</t>
+  </si>
+  <si>
+    <t>You need to be in the participants list, quando a tarefa dava a entender que era para os participants serem apenas aqueles dois, e meio que encravou porque a informação era contraditória. Fez a reserva para o dia errado mas por ler mal a tarefa.</t>
+  </si>
+  <si>
+    <t>Tempo</t>
+  </si>
+  <si>
+    <t>Percebeu bem qual era a segunda sessão, mas não percebeu que só via as suas sessões</t>
+  </si>
+  <si>
+    <t>Pôr o calendário a começar na segunda feira e mostrar fins de semana com cores diferentes.</t>
+  </si>
+  <si>
+    <t>Ler o calendario. Ficou confuso ao escolher os karts mas percebeu sozinho que os participants tinham de ter karts diferentes.</t>
+  </si>
+  <si>
+    <t>Demorou mais a pensar como escrever o que queria em inglês, não era necessário.</t>
+  </si>
+  <si>
+    <t>Erro de implementacao</t>
+  </si>
+  <si>
+    <t>Organizar melhor as sessões para não ficar confuso, possivelmente estarem dentro de cada track</t>
+  </si>
+  <si>
+    <t>Encontrou a enterprise view muito rápido.</t>
+  </si>
+  <si>
+    <t>Não gostou do owner tambem ter acesso as funcionalidades de cliente. Disse não fazer sentido caso a conta seja usada num computador geral na pista, com qualquer funcionário a ter acesso.</t>
+  </si>
+  <si>
+    <t>Erro de implementação ao rejeitar a reserva, não relacionado com a reserva</t>
+  </si>
+  <si>
+    <t>Demorou um pouco a encontrar a enterprise view.</t>
+  </si>
+  <si>
+    <t>Médio</t>
+  </si>
+  <si>
+    <t>Se mantivermos as contas com as duas vistas, podíamos ter uma página após o login para escolher em qual vista entrar</t>
+  </si>
+  <si>
+    <t>Quis fazer mais do que o pedido então foi procurar reservas noutras pistas. Achou que não podia cancelar uma reserva que tinha sido aceite.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +196,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -111,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -134,25 +246,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{54E39800-220E-45D3-8955-47691E231D79}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -454,19 +632,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="5" max="5" width="59" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -474,80 +652,89 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2"/>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -556,19 +743,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707F8221-5F9C-48B8-9438-2F610B15D8CA}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="54.42578125" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" customWidth="1"/>
+    <col min="5" max="5" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -576,80 +763,84 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -661,16 +852,16 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="59" customWidth="1"/>
+    <col min="5" max="5" width="76.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,80 +869,110 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -760,19 +981,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C37D6F-40A2-4651-B3C5-7BD0EECD8CDB}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60" customWidth="1"/>
+    <col min="5" max="5" width="65.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -780,90 +1001,333 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B1E082-59F4-4254-BB75-63E2DABD758B}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="4" max="4" width="63.28515625" customWidth="1"/>
+    <col min="5" max="5" width="69.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CF512E-C7FC-4ADD-868F-728C7A948E1F}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
+      <c r="B10" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>